<commit_message>
Final state of the sourcecode
</commit_message>
<xml_diff>
--- a/sourcecode/webscraper/Abbreviations.xlsx
+++ b/sourcecode/webscraper/Abbreviations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonia/Desktop/Masterprojekt/Repository/sourcecode/webscraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BFF990-8D24-014B-AE5B-DCC4425636D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A697B1-96CB-B742-8BF6-8DA3A153EAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-260" yWindow="-19180" windowWidth="28240" windowHeight="16540" xr2:uid="{E4C02291-2958-A243-B102-A950122962A1}"/>
+    <workbookView xWindow="1640" yWindow="1320" windowWidth="28240" windowHeight="16540" xr2:uid="{E4C02291-2958-A243-B102-A950122962A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -153,9 +153,6 @@
     <t>Swedish</t>
   </si>
   <si>
-    <t>Dansk</t>
-  </si>
-  <si>
     <t>Slovenian</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>Version 2</t>
+  </si>
+  <si>
+    <t>Danish</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,13 +570,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>

</xml_diff>